<commit_message>
Atualiza parcial e avisos da Liga Eliminacao 20
</commit_message>
<xml_diff>
--- a/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao_20.xlsx
+++ b/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao_20.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Time</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Rodada 19</t>
+  </si>
+  <si>
+    <t>Parcial Rodada 1</t>
   </si>
   <si>
     <t>time_id</t>
@@ -494,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -564,225 +567,288 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>32966</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2">
+        <v>44.26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>184499</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>186283</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4">
+        <v>45.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1">
         <v>287965</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5">
+        <v>58.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1">
         <v>1273719</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6">
+        <v>59.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1">
         <v>1326835</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7">
+        <v>16.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>1488983</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="V8">
+        <v>38.46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>1747619</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9">
+        <v>39.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>1867254</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="V10">
+        <v>55.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>2371918</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11">
+        <v>63.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1">
         <v>2916559</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="V12">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1">
         <v>4088673</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="V13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1">
         <v>14709358</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14">
+        <v>67.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1">
         <v>14933455</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15">
+        <v>53.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1">
         <v>16411206</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="V16">
+        <v>44.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="1">
         <v>19209079</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="V17">
+        <v>62.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="1">
         <v>19833277</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="V18">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="1">
         <v>20651178</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="V19">
+        <v>52.66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="1">
         <v>44810918</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="V20">
+        <v>54.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="1">
         <v>47775950</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>0</v>
+      </c>
+      <c r="V21">
+        <v>53.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>